<commit_message>
Updated BOM and added slight improvements to the PCB layout.
</commit_message>
<xml_diff>
--- a/eagle/Bill of Materials.xlsx
+++ b/eagle/Bill of Materials.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16540" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="75">
   <si>
     <t>Description</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Mouser Unit Cost</t>
   </si>
   <si>
-    <t>DigiKey Unit Cost</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -105,15 +102,6 @@
     <t>U.FL RECEPTACLE SMT</t>
   </si>
   <si>
-    <t>Mouser Cost</t>
-  </si>
-  <si>
-    <t>DigiKey Cost</t>
-  </si>
-  <si>
-    <t>Total Cost Minimized Cost:</t>
-  </si>
-  <si>
     <t>59-LTST-C230KGKT</t>
   </si>
   <si>
@@ -132,17 +120,141 @@
     <t>660-RK73H2BTTD1001F</t>
   </si>
   <si>
-    <t>SMD 1206 1/4watts 1Kohms 1%</t>
+    <t>Stackable Header - 2x23 Pin Female</t>
+  </si>
+  <si>
+    <t>485-706</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>DHT22 Temp/Humidity Sensor</t>
+  </si>
+  <si>
+    <t>485-385</t>
+  </si>
+  <si>
+    <t>PMS3003 Wire Housing</t>
+  </si>
+  <si>
+    <t>53261-0871</t>
+  </si>
+  <si>
+    <t>538-53261-0871</t>
+  </si>
+  <si>
+    <t>WM7626DKR-ND</t>
+  </si>
+  <si>
+    <t>SMD 1206 1/4watt 1Kohms 1%</t>
+  </si>
+  <si>
+    <t>SMD 1206 1/4watt 82ohms 1% by Vishay</t>
+  </si>
+  <si>
+    <t>CRCW120682R0FKEA</t>
+  </si>
+  <si>
+    <t>71-CRCW1206-82-E3</t>
+  </si>
+  <si>
+    <t>541-82.0FCT-ND</t>
+  </si>
+  <si>
+    <t>SMD 1206 1/4watt 51ohms 1% by Vishay</t>
+  </si>
+  <si>
+    <t>CRCW120651R0FKEA</t>
+  </si>
+  <si>
+    <t>71-CRCW1206-51-E3</t>
+  </si>
+  <si>
+    <t>541-51.0UCT-ND</t>
+  </si>
+  <si>
+    <t>SMD 1206 1/4watt 22kohms 1% by Vishay</t>
+  </si>
+  <si>
+    <t>CRCW120622K0FKEA</t>
+  </si>
+  <si>
+    <t>71-CRCW1206-22K-E3</t>
+  </si>
+  <si>
+    <t>541-22.0KFCT-ND</t>
+  </si>
+  <si>
+    <t>SMD 1206 1/4watt 47kohms 1% by Vishay</t>
+  </si>
+  <si>
+    <t>CRCW120647K0FKEA</t>
+  </si>
+  <si>
+    <t>71-CRCW1206-47K-E3</t>
+  </si>
+  <si>
+    <t>541-47.0KUCT-ND</t>
+  </si>
+  <si>
+    <t>N-Channel MOSFET</t>
+  </si>
+  <si>
+    <t>BSS138LT1G</t>
+  </si>
+  <si>
+    <t>863-BSS138LT1G</t>
+  </si>
+  <si>
+    <t>BSS138LT1GOSCT-ND</t>
+  </si>
+  <si>
+    <t>Ferrite Bead</t>
+  </si>
+  <si>
+    <t>MMZ2012R102A</t>
+  </si>
+  <si>
+    <t>810-MMZ2012R102A</t>
+  </si>
+  <si>
+    <t>445-1555-1-ND</t>
+  </si>
+  <si>
+    <t>MICS 4514 (CO/NO2) Sensor</t>
+  </si>
+  <si>
+    <t>MICS-4514</t>
+  </si>
+  <si>
+    <t>MTK3339 GPS Chipset</t>
+  </si>
+  <si>
+    <t>Ultimate GPS Module</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>OSH Park PCBs</t>
+  </si>
+  <si>
+    <t>Total Estimated Cost</t>
+  </si>
+  <si>
+    <t>$13 per board</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -178,11 +290,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="12"/>
@@ -225,18 +332,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -572,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -588,11 +695,13 @@
     <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -605,7 +714,7 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -618,21 +727,16 @@
         <v>10</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -641,287 +745,581 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2" s="4">
         <v>3.698</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="3">
+      <c r="I2" s="3">
         <f>B2*H2</f>
-        <v>73.959999999999994</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="9" t="s">
+        <v>3.698</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8">
+        <v>385</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="I3" s="3">
+        <f>B3*H3</f>
+        <v>9.9499999999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="3">
+        <v>9.7200000000000006</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" ref="I4:I5" si="0">B4*H4</f>
+        <v>9.7200000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="3">
+        <v>29.95</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="0"/>
+        <v>29.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1.2929999999999999</v>
+      </c>
+      <c r="I8" s="3">
+        <f>B8*H8</f>
+        <v>1.2929999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B3">
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="I9" s="3">
+        <f>B9*H9</f>
+        <v>0.63700000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1.82</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" ref="I10:I12" si="1">B10*H10</f>
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" s="8">
+        <v>706</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="3">
+        <v>4.95</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="1"/>
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="1"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0.373</v>
+      </c>
+      <c r="I14" s="3">
+        <f>B14*H14</f>
+        <v>1.492</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="H15" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" ref="I15:I19" si="2">B15*H15</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="I21" s="3">
+        <f>B21*H21</f>
+        <v>1.071</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="3">
-        <v>1.2929999999999999</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" ref="J3:J10" si="0">B3*H3</f>
-        <v>25.86</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4">
-        <v>20</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0.63700000000000001</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0.63700000000000001</v>
-      </c>
-      <c r="J4" s="3">
-        <f t="shared" si="0"/>
-        <v>12.74</v>
-      </c>
-      <c r="K4" s="3">
-        <f>B4*I4</f>
-        <v>12.74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="10"/>
-      <c r="J5" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <f t="shared" ref="K5:K6" si="1">B5*I5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="10"/>
-      <c r="J6" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7">
+      <c r="E22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="I22" s="3">
+        <f>B22*H22</f>
+        <v>0.55300000000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="4">
-        <v>0.373</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0.80200000000000005</v>
-      </c>
-      <c r="J7" s="3">
-        <f t="shared" si="0"/>
-        <v>22.38</v>
-      </c>
-      <c r="K7" s="3">
-        <f>B7*I7</f>
-        <v>48.120000000000005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8">
-        <v>20</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9">
-        <v>60</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0.35699999999999998</v>
-      </c>
-      <c r="I9" s="5">
-        <v>0.253</v>
-      </c>
-      <c r="J9" s="3">
-        <f t="shared" si="0"/>
-        <v>21.419999999999998</v>
-      </c>
-      <c r="K9" s="3">
-        <f>B9*I9</f>
-        <v>15.18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10">
-        <v>20</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="4">
-        <v>0.55300000000000005</v>
-      </c>
-      <c r="I10" s="5">
-        <v>0.68400000000000005</v>
-      </c>
-      <c r="J10" s="3">
-        <f t="shared" si="0"/>
-        <v>11.06</v>
-      </c>
-      <c r="K10" s="3">
-        <f>B10*I10</f>
-        <v>13.680000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="10"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="10"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="3">
-        <f>J2+J3+J7+K9+J10</f>
-        <v>148.44</v>
+      <c r="D24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0.24</v>
+      </c>
+      <c r="I24" s="3">
+        <f>B24*H24</f>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" s="9">
+        <v>38</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="3">
+        <f>SUM(I2:I24)+13</f>
+        <v>84.033999999999978</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="C7" r:id="rId2"/>
-    <hyperlink ref="D7" r:id="rId3" tooltip="Click to view additional information on this product."/>
-    <hyperlink ref="E7" r:id="rId4"/>
-    <hyperlink ref="E9" r:id="rId5"/>
-    <hyperlink ref="C9" r:id="rId6"/>
-    <hyperlink ref="D9" r:id="rId7"/>
-    <hyperlink ref="C10" r:id="rId8"/>
-    <hyperlink ref="D10" r:id="rId9" tooltip="Click to view additional information on this product."/>
-    <hyperlink ref="E10" r:id="rId10"/>
-    <hyperlink ref="C3" r:id="rId11" tooltip="Click to view additional information on this product."/>
-    <hyperlink ref="D3" r:id="rId12"/>
-    <hyperlink ref="C4" r:id="rId13" tooltip="Click to view additional information on this product."/>
-    <hyperlink ref="D4" r:id="rId14"/>
-    <hyperlink ref="E4" r:id="rId15"/>
-    <hyperlink ref="C8" r:id="rId16"/>
-    <hyperlink ref="D8" r:id="rId17" tooltip="Click to view additional information on this product."/>
+    <hyperlink ref="C14" r:id="rId2"/>
+    <hyperlink ref="D14" r:id="rId3" tooltip="Click to view additional information on this product."/>
+    <hyperlink ref="E14" r:id="rId4"/>
+    <hyperlink ref="E21" r:id="rId5"/>
+    <hyperlink ref="C21" r:id="rId6"/>
+    <hyperlink ref="D21" r:id="rId7"/>
+    <hyperlink ref="C22" r:id="rId8"/>
+    <hyperlink ref="D22" r:id="rId9" tooltip="Click to view additional information on this product."/>
+    <hyperlink ref="E22" r:id="rId10"/>
+    <hyperlink ref="C8" r:id="rId11" tooltip="Click to view additional information on this product."/>
+    <hyperlink ref="D8" r:id="rId12"/>
+    <hyperlink ref="C9" r:id="rId13" tooltip="Click to view additional information on this product."/>
+    <hyperlink ref="D9" r:id="rId14"/>
+    <hyperlink ref="E9" r:id="rId15"/>
+    <hyperlink ref="C15" r:id="rId16"/>
+    <hyperlink ref="D15" r:id="rId17" tooltip="Click to view additional information on this product."/>
+    <hyperlink ref="D11" r:id="rId18"/>
+    <hyperlink ref="C11" r:id="rId19" display="https://www.adafruit.com/products/706"/>
+    <hyperlink ref="D3" r:id="rId20"/>
+    <hyperlink ref="C3" r:id="rId21" display="https://www.adafruit.com/products/385"/>
+    <hyperlink ref="C10" r:id="rId22"/>
+    <hyperlink ref="D10" r:id="rId23"/>
+    <hyperlink ref="E10" r:id="rId24"/>
+    <hyperlink ref="C16" r:id="rId25"/>
+    <hyperlink ref="D16" r:id="rId26"/>
+    <hyperlink ref="E16" r:id="rId27"/>
+    <hyperlink ref="C17" r:id="rId28"/>
+    <hyperlink ref="D17" r:id="rId29"/>
+    <hyperlink ref="E17" r:id="rId30"/>
+    <hyperlink ref="C18" r:id="rId31"/>
+    <hyperlink ref="D18" r:id="rId32"/>
+    <hyperlink ref="E18" r:id="rId33"/>
+    <hyperlink ref="C19" r:id="rId34"/>
+    <hyperlink ref="D19" r:id="rId35"/>
+    <hyperlink ref="E19" r:id="rId36"/>
+    <hyperlink ref="C24" r:id="rId37"/>
+    <hyperlink ref="D24" r:id="rId38"/>
+    <hyperlink ref="E24" r:id="rId39"/>
+    <hyperlink ref="C12" r:id="rId40"/>
+    <hyperlink ref="D12" r:id="rId41"/>
+    <hyperlink ref="E12" r:id="rId42"/>
+    <hyperlink ref="C4" r:id="rId43" location=".Vo1CYZMrJp8"/>
+    <hyperlink ref="C5" r:id="rId44"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added board layout PDF and manufacturing checklist
</commit_message>
<xml_diff>
--- a/eagle/Bill of Materials.xlsx
+++ b/eagle/Bill of Materials.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27106"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="1460" windowWidth="25600" windowHeight="16540" tabRatio="500"/>
+    <workbookView xWindow="3200" yWindow="480" windowWidth="25600" windowHeight="16540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -766,7 +766,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:I27"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1157,7 +1157,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>12</v>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="I17" s="17">
         <f>B17*H17</f>
-        <v>1.492</v>
+        <v>1.865</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1494,7 +1494,7 @@
       </c>
       <c r="B34" s="3">
         <f>SUM(I2:I29)+13</f>
-        <v>80.813999999999965</v>
+        <v>81.186999999999955</v>
       </c>
     </row>
   </sheetData>

</xml_diff>